<commit_message>
wrote support functions for team_page
</commit_message>
<xml_diff>
--- a/2020Data.xlsx
+++ b/2020Data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC53"/>
+  <dimension ref="A1:AD57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,6 +508,11 @@
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>fortune wheel</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>shootPlace2</t>
         </is>
@@ -581,6 +586,7 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -650,6 +656,7 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -715,6 +722,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -780,6 +788,7 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -845,6 +854,7 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -906,6 +916,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -956,6 +967,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1025,6 +1037,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1080,6 +1093,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1153,6 +1167,7 @@
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1218,6 +1233,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1271,6 +1287,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1344,6 +1361,7 @@
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1417,63 +1435,60 @@
         </is>
       </c>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>111</v>
+        <v>4590</v>
       </c>
       <c r="B16" t="n">
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Two</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>attacked</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nope</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>lift 1</t>
-        </is>
-      </c>
+          <t>autoCell</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>0</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Starting balls</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1483,27 +1498,20 @@
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>Trench</t>
-        </is>
-      </c>
+      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>Trench+Other</t>
-        </is>
-      </c>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>444</v>
+        <v>4590</v>
       </c>
       <c r="B17" t="n">
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1511,7 +1519,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1525,22 +1533,22 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Floor</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>attacked</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>shutdown</t>
+          <t>nope</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>lift 2</t>
+          <t>lift 0</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1562,70 +1570,75 @@
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Trench</t>
         </is>
       </c>
       <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>no can do</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B18" t="n">
         <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>autonomous</t>
+          <t>teleop</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>autoCell</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Two</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>attacked</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nope</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>lift 1</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
         <v>0</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Starting balls</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
@@ -1633,68 +1646,77 @@
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>Trench</t>
+        </is>
+      </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>Trench+Other</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B19" t="n">
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>autonomous</t>
+          <t>teleop</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>autoCell</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Floor</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>attacked</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>shutdown</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>lift 2</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>64</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>Starting balls</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
@@ -1702,9 +1724,14 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1714,56 +1741,56 @@
         <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Zero</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>was attacked</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>shutdown</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>lift 0</t>
-        </is>
-      </c>
+          <t>autoCell</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
         <v>0</v>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Starting balls</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
@@ -1774,16 +1801,17 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B21" t="n">
         <v>3</v>
       </c>
       <c r="C21" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1791,7 +1819,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1805,11 +1833,11 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Picked up</t>
+          <t>Starting balls</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -1819,18 +1847,18 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -1843,6 +1871,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1852,50 +1881,54 @@
         <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>autonomous</t>
+          <t>teleop</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>autoCell</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Zero</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>was attacked</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>shutdown</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>lift 0</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
         <v>0</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>Starting balls</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1908,28 +1941,29 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B23" t="n">
         <v>3</v>
       </c>
       <c r="C23" t="n">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Climb</t>
+          <t>autoCell</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1941,38 +1975,43 @@
       <c r="M23" t="n">
         <v>0</v>
       </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Picked up</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>UnBalanced</t>
-        </is>
-      </c>
-      <c r="W23" t="n">
-        <v>91</v>
-      </c>
-      <c r="X23" t="n">
-        <v>0</v>
-      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1982,19 +2021,19 @@
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PowerCells</t>
+          <t>autoCell</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -2006,7 +2045,11 @@
       <c r="M24" t="n">
         <v>0</v>
       </c>
-      <c r="N24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Starting balls</t>
+        </is>
+      </c>
       <c r="O24" t="inlineStr">
         <is>
           <t>Low</t>
@@ -2014,12 +2057,12 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="R24" t="inlineStr"/>
@@ -2034,16 +2077,17 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B25" t="n">
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2051,7 +2095,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2078,33 +2122,52 @@
           <t>2nd</t>
         </is>
       </c>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>UnBalanced</t>
+        </is>
+      </c>
       <c r="W25" t="n">
-        <v>147</v>
-      </c>
-      <c r="X25" t="inlineStr"/>
+        <v>91</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B26" t="n">
         <v>3</v>
       </c>
       <c r="C26" t="n">
-        <v>91</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
       <c r="E26" t="n">
-        <v>91</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>PowerCells</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
@@ -2115,9 +2178,21 @@
         <v>0</v>
       </c>
       <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2125,32 +2200,22 @@
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>שיהיה לך סרטן בזין
-שיהיה לך סרטן בביצים
-ולא תוכל לזיין ותמות
-אמן כן כיהיה רצון!!!!!!</t>
-        </is>
-      </c>
-      <c r="Z26" t="inlineStr">
-        <is>
-          <t>houston</t>
-        </is>
-      </c>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B27" t="n">
         <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2158,11 +2223,11 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>PowerCells</t>
+          <t>Climb</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -2175,33 +2240,28 @@
         <v>0</v>
       </c>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
+      <c r="W27" t="n">
+        <v>147</v>
+      </c>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2240,7 +2300,10 @@
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>LOVE YOU ROEKY</t>
+          <t>שיהיה לך סרטן בזין
+שיהיה לך סרטן בביצים
+ולא תוכל לזיין ותמות
+אמן כן כיהיה רצון!!!!!!</t>
         </is>
       </c>
       <c r="Z28" t="inlineStr">
@@ -2251,6 +2314,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2272,42 +2336,34 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>One</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Feeder</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>was attacked</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>nope</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>lift 1</t>
-        </is>
-      </c>
+          <t>PowerCells</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
         <v>0</v>
       </c>
       <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2318,36 +2374,25 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="inlineStr"/>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>Wall</t>
-        </is>
-      </c>
+      <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B30" t="n">
         <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>11</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>autonomous</t>
-        </is>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>11</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>autoCell</t>
-        </is>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
@@ -2357,60 +2402,49 @@
       <c r="M30" t="n">
         <v>0</v>
       </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>Picked up</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>LOVE YOU ROEKY</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>houston</t>
+        </is>
+      </c>
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>444</v>
+        <v>4590</v>
       </c>
       <c r="B31" t="n">
         <v>3</v>
       </c>
       <c r="C31" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>autonomous</t>
+          <t>teleop</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2438,12 +2472,12 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R31" t="inlineStr"/>
@@ -2458,6 +2492,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2479,40 +2514,44 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>PowerCells</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>One</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Feeder</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>was attacked</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>nope</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>lift 1</t>
+        </is>
+      </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
         <v>0</v>
       </c>
       <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
@@ -2521,8 +2560,13 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr"/>
-      <c r="AB32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>Wall</t>
+        </is>
+      </c>
       <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2532,19 +2576,19 @@
         <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Climb</t>
+          <t>autoCell</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2556,38 +2600,43 @@
       <c r="M33" t="n">
         <v>0</v>
       </c>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Picked up</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V33" t="inlineStr">
-        <is>
-          <t>UnBalanced</t>
-        </is>
-      </c>
-      <c r="W33" t="n">
-        <v>147</v>
-      </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2597,19 +2646,19 @@
         <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Climb</t>
+          <t>autoCell</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2621,48 +2670,49 @@
       <c r="M34" t="n">
         <v>0</v>
       </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Picked up</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>Balanced</t>
-        </is>
-      </c>
-      <c r="W34" t="n">
-        <v>70</v>
-      </c>
-      <c r="X34" t="n">
-        <v>0</v>
-      </c>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr"/>
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B35" t="n">
         <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2670,7 +2720,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2689,21 +2739,25 @@
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
@@ -2714,6 +2768,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr"/>
       <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2735,7 +2790,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>PowerCells</t>
+          <t>Climb</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2748,33 +2803,38 @@
         <v>0</v>
       </c>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr"/>
-      <c r="X36" t="inlineStr"/>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>UnBalanced</t>
+        </is>
+      </c>
+      <c r="W36" t="n">
+        <v>147</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr"/>
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr"/>
       <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2784,7 +2844,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="n">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2792,7 +2852,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2816,36 +2876,55 @@
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr">
         <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
       <c r="W37" t="n">
-        <v>147</v>
-      </c>
-      <c r="X37" t="inlineStr"/>
+        <v>70</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr"/>
       <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B38" t="n">
         <v>3</v>
       </c>
       <c r="C38" t="n">
-        <v>91</v>
-      </c>
-      <c r="D38" t="inlineStr"/>
+        <v>147</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
       <c r="E38" t="n">
-        <v>91</v>
-      </c>
-      <c r="F38" t="inlineStr"/>
+        <v>147</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>PowerCells</t>
+        </is>
+      </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
@@ -2856,9 +2935,21 @@
         <v>0</v>
       </c>
       <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
@@ -2866,37 +2957,36 @@
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>יואווווווווו
-כמה כוסית עדי הימלבלוי
-אני מפליץ מרוב התרגשות</t>
-        </is>
-      </c>
-      <c r="Z38" t="inlineStr">
-        <is>
-          <t>houston</t>
-        </is>
-      </c>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr"/>
       <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B39" t="n">
         <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>91</v>
-      </c>
-      <c r="D39" t="inlineStr"/>
+        <v>147</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
       <c r="E39" t="n">
-        <v>91</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
+        <v>147</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>PowerCells</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
@@ -2907,9 +2997,21 @@
         <v>0</v>
       </c>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
@@ -2917,29 +3019,22 @@
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>ITAI GIL IS BIG DADDY UWU</t>
-        </is>
-      </c>
-      <c r="Z39" t="inlineStr">
-        <is>
-          <t>houston</t>
-        </is>
-      </c>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
       <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B40" t="n">
         <v>3</v>
       </c>
       <c r="C40" t="n">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2947,7 +3042,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2971,13 +3066,13 @@
       <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr">
         <is>
-          <t>2nd</t>
+          <t>1st</t>
         </is>
       </c>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
       <c r="W40" t="n">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr"/>
@@ -2985,30 +3080,23 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr"/>
       <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>666</v>
+        <v>111</v>
       </c>
       <c r="B41" t="n">
         <v>3</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>autonomous</t>
-        </is>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>autoCell</t>
-        </is>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
@@ -3018,42 +3106,33 @@
       <c r="M41" t="n">
         <v>0</v>
       </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>Picked up</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
       <c r="W41" t="inlineStr"/>
       <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>יואווווווווו
+כמה כוסית עדי הימלבלוי
+אני מפליץ מרוב התרגשות</t>
+        </is>
+      </c>
+      <c r="Z41" t="inlineStr">
+        <is>
+          <t>houston</t>
+        </is>
+      </c>
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="inlineStr"/>
+      <c r="AD41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3065,44 +3144,16 @@
       <c r="C42" t="n">
         <v>91</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>teleop</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
         <v>91</v>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Two</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Floor</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>was attacked</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>shutdown</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>lift 2</t>
-        </is>
-      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="n">
         <v>0</v>
@@ -3118,19 +3169,20 @@
       <c r="V42" t="inlineStr"/>
       <c r="W42" t="inlineStr"/>
       <c r="X42" t="inlineStr"/>
-      <c r="Y42" t="inlineStr"/>
-      <c r="Z42" t="inlineStr"/>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>ITAI GIL IS BIG DADDY UWU</t>
+        </is>
+      </c>
+      <c r="Z42" t="inlineStr">
+        <is>
+          <t>houston</t>
+        </is>
+      </c>
+      <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr"/>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>Wall+Trench</t>
-        </is>
-      </c>
+      <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3152,34 +3204,14 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>attacked</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>shutdown</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>lift 2</t>
-        </is>
-      </c>
+          <t>Climb</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
         <v>0</v>
@@ -3190,79 +3222,82 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr"/>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
+      <c r="W43" t="n">
+        <v>91</v>
+      </c>
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>Wall</t>
-        </is>
-      </c>
+      <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>444</v>
+        <v>666</v>
       </c>
       <c r="B44" t="n">
         <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>teleop</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>attacked</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>nope</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>lift 2</t>
-        </is>
-      </c>
+          <t>autoCell</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="n">
         <v>0</v>
       </c>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Picked up</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr"/>
@@ -3270,13 +3305,10 @@
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" t="inlineStr"/>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>Wall</t>
-        </is>
-      </c>
+      <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3303,27 +3335,27 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>One</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Floor</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>attacked</t>
+          <t>was attacked</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>nope</t>
+          <t>shutdown</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>lift 1</t>
+          <t>lift 2</t>
         </is>
       </c>
       <c r="L45" t="inlineStr"/>
@@ -3343,23 +3375,28 @@
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="inlineStr"/>
-      <c r="AA45" t="inlineStr"/>
-      <c r="AB45" t="inlineStr">
-        <is>
-          <t>Trench</t>
-        </is>
-      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AB45" t="inlineStr"/>
       <c r="AC45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>Wall+Trench</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B46" t="n">
         <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3367,44 +3404,48 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>PowerCells</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>attacked</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>shutdown</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>lift 2</t>
+        </is>
+      </c>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="n">
         <v>0</v>
       </c>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
@@ -3412,19 +3453,24 @@
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="inlineStr"/>
-      <c r="AA46" t="inlineStr"/>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>Wall</t>
+        </is>
+      </c>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B47" t="n">
         <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3432,44 +3478,48 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>PowerCells</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>attacked</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>nope</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>lift 2</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="n">
         <v>0</v>
       </c>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
@@ -3477,19 +3527,24 @@
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr"/>
-      <c r="AA47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>Wall</t>
+        </is>
+      </c>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="B48" t="n">
         <v>3</v>
       </c>
       <c r="C48" t="n">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -3497,18 +3552,38 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Climb</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>One</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>attacked</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>nope</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>lift 1</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="n">
         <v>0</v>
@@ -3519,42 +3594,31 @@
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr"/>
-      <c r="T48" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V48" t="inlineStr">
-        <is>
-          <t>UnBalanced</t>
-        </is>
-      </c>
-      <c r="W48" t="n">
-        <v>37</v>
-      </c>
-      <c r="X48" t="n">
-        <v>0</v>
-      </c>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
       <c r="Y48" t="inlineStr"/>
       <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr"/>
-      <c r="AB48" t="inlineStr"/>
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t>Trench</t>
+        </is>
+      </c>
       <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B49" t="n">
         <v>3</v>
       </c>
       <c r="C49" t="n">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -3562,11 +3626,11 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Climb</t>
+          <t>PowerCells</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -3579,37 +3643,38 @@
         <v>0</v>
       </c>
       <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
-      <c r="T49" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V49" t="inlineStr">
-        <is>
-          <t>UnBalanced</t>
-        </is>
-      </c>
-      <c r="W49" t="n">
-        <v>91</v>
-      </c>
-      <c r="X49" t="n">
-        <v>0</v>
-      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
       <c r="AC49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3631,7 +3696,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Climb</t>
+          <t>PowerCells</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3644,47 +3709,48 @@
         <v>0</v>
       </c>
       <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
-      <c r="T50" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>Balanced</t>
-        </is>
-      </c>
-      <c r="W50" t="n">
-        <v>91</v>
-      </c>
-      <c r="X50" t="n">
-        <v>0</v>
-      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>111</v>
+        <v>444</v>
       </c>
       <c r="B51" t="n">
         <v>3</v>
       </c>
       <c r="C51" t="n">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -3692,11 +3758,11 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>PowerCells</t>
+          <t>Climb</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3709,43 +3775,48 @@
         <v>0</v>
       </c>
       <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr"/>
-      <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
-      <c r="W51" t="inlineStr"/>
-      <c r="X51" t="inlineStr"/>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>UnBalanced</t>
+        </is>
+      </c>
+      <c r="W51" t="n">
+        <v>37</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0</v>
+      </c>
       <c r="Y51" t="inlineStr"/>
       <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>666</v>
+        <v>111</v>
       </c>
       <c r="B52" t="n">
         <v>3</v>
       </c>
       <c r="C52" t="n">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -3753,7 +3824,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3780,27 +3851,38 @@
           <t>2nd</t>
         </is>
       </c>
-      <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>UnBalanced</t>
+        </is>
+      </c>
       <c r="W52" t="n">
-        <v>26</v>
-      </c>
-      <c r="X52" t="inlineStr"/>
+        <v>91</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
       <c r="Y52" t="inlineStr"/>
       <c r="Z52" t="inlineStr"/>
       <c r="AA52" t="inlineStr"/>
       <c r="AB52" t="inlineStr"/>
       <c r="AC52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>666</v>
+        <v>111</v>
       </c>
       <c r="B53" t="n">
         <v>3</v>
       </c>
       <c r="C53" t="n">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -3808,11 +3890,11 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>PowerCells</t>
+          <t>Climb</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3825,33 +3907,288 @@
         <v>0</v>
       </c>
       <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr"/>
-      <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="W53" t="n">
+        <v>91</v>
+      </c>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr"/>
       <c r="AA53" t="inlineStr"/>
       <c r="AB53" t="inlineStr"/>
       <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>111</v>
+      </c>
+      <c r="B54" t="n">
+        <v>3</v>
+      </c>
+      <c r="C54" t="n">
+        <v>91</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>91</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>PowerCells</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>666</v>
+      </c>
+      <c r="B55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C55" t="n">
+        <v>26</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>26</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Climb</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="n">
+        <v>26</v>
+      </c>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>666</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" t="n">
+        <v>26</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>teleop</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>26</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>PowerCells</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>4590</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3</v>
+      </c>
+      <c r="C57" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>autonomous</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>autoCell</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="n">
+        <v>3</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>Starting balls</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
added game page with functions to get teams in game
</commit_message>
<xml_diff>
--- a/2020Data.xlsx
+++ b/2020Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GreenBlitz\PycharmProjects\scouting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF35E4-F215-43E2-9017-F10724B604A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1523653E-BB2A-4FC9-A7C8-89260D47F2DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="80">
   <si>
     <t>teamNumber</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>teamPageNumber</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,6 +1054,9 @@
       <c r="T10" t="s">
         <v>49</v>
       </c>
+      <c r="U10" t="s">
+        <v>50</v>
+      </c>
       <c r="W10">
         <v>37</v>
       </c>
@@ -1355,6 +1361,9 @@
       <c r="AA18" t="s">
         <v>59</v>
       </c>
+      <c r="AC18" t="s">
+        <v>79</v>
+      </c>
       <c r="AD18" t="s">
         <v>67</v>
       </c>
@@ -2714,5 +2723,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added pie chart for shutdown and bar chart for fortune wheel to power bi
</commit_message>
<xml_diff>
--- a/2020Data.xlsx
+++ b/2020Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GreenBlitz\PycharmProjects\scouting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1523653E-BB2A-4FC9-A7C8-89260D47F2DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0659418-6E13-49BF-8407-5526DFD1AE27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="81">
   <si>
     <t>teamNumber</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>aa</t>
+  </si>
+  <si>
+    <t>rotation control</t>
   </si>
 </sst>
 </file>
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -786,6 +789,9 @@
       <c r="M2">
         <v>0</v>
       </c>
+      <c r="AC2" t="s">
+        <v>80</v>
+      </c>
       <c r="AE2">
         <v>111</v>
       </c>

</xml_diff>